<commit_message>
version send to co-authors
version send to co-authors - minor updates
</commit_message>
<xml_diff>
--- a/results/Models/Table_models_MEP.xlsx
+++ b/results/Models/Table_models_MEP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helsinkifi-my.sharepoint.com/personal/beckeant_ad_helsinki_fi/Documents/ABS_Postdoc/Helsinki/Work/Arctic_Flowering/Zackenberg_Flowering/results/Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beckeant/Library/CloudStorage/OneDrive-UniversityofHelsinki/ABS_Postdoc/Helsinki/Work/Arctic_Flowering/Zackenberg_Flowering/results/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="993" documentId="13_ncr:1_{1B0DA5C5-DF59-1644-BB10-405D1AEC11DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF761176-BC80-D848-98AB-0855D1FE2DB6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D963F0-84F9-6D45-8769-7E8B137B3587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5720" yWindow="-21100" windowWidth="37360" windowHeight="21100" activeTab="3" xr2:uid="{21647BD2-5D45-904F-BF0E-D57BB03BEE0E}"/>
+    <workbookView xWindow="-5720" yWindow="-21100" windowWidth="18000" windowHeight="21100" activeTab="3" xr2:uid="{21647BD2-5D45-904F-BF0E-D57BB03BEE0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Study_design" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="593">
   <si>
     <t>Predictors</t>
   </si>
@@ -1818,9 +1818,6 @@
     <t>0.549</t>
   </si>
   <si>
-    <t>-0.00</t>
-  </si>
-  <si>
     <t>-0.24 – 0.23</t>
   </si>
   <si>
@@ -1972,36 +1969,6 @@
   </si>
   <si>
     <t>3.09</t>
-  </si>
-  <si>
-    <r>
-      <t>490 </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Plot</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>54 </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>Plot</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2037,12 +2004,15 @@
       <t>2</t>
     </r>
   </si>
+  <si>
+    <t>54</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2268,13 +2238,6 @@
       <family val="1"/>
     </font>
     <font>
-      <vertAlign val="subscript"/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
       <vertAlign val="superscript"/>
       <sz val="14"/>
       <color theme="1"/>
@@ -2361,7 +2324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2713,24 +2676,6 @@
     <xf numFmtId="0" fontId="33" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2788,16 +2733,16 @@
     <xf numFmtId="2" fontId="23" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="36" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="35" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="27" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2812,13 +2757,37 @@
     <xf numFmtId="2" fontId="31" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="28" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3309,23 +3278,23 @@
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="129" t="s">
+      <c r="C2" s="159" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="129" t="s">
+      <c r="K2" s="159" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
       <c r="P2" s="12"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
@@ -4736,19 +4705,19 @@
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="37"/>
-      <c r="E3" s="130" t="s">
+      <c r="E3" s="160" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
       <c r="I3" s="38"/>
-      <c r="J3" s="130" t="s">
+      <c r="J3" s="160" t="s">
         <v>118</v>
       </c>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
       <c r="N3" s="35"/>
     </row>
     <row r="4" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4858,19 +4827,19 @@
       <c r="D7" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="131" t="s">
+      <c r="E7" s="161" t="s">
         <v>200</v>
       </c>
-      <c r="F7" s="131"/>
-      <c r="G7" s="131"/>
-      <c r="H7" s="131"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="161"/>
+      <c r="H7" s="161"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="131" t="s">
+      <c r="J7" s="161" t="s">
         <v>126</v>
       </c>
-      <c r="K7" s="131"/>
-      <c r="L7" s="131"/>
-      <c r="M7" s="131"/>
+      <c r="K7" s="161"/>
+      <c r="L7" s="161"/>
+      <c r="M7" s="161"/>
       <c r="N7" s="35"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -5107,10 +5076,10 @@
         <v>66</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
+      <c r="C12" s="162"/>
+      <c r="D12" s="162"/>
+      <c r="E12" s="162"/>
+      <c r="F12" s="162"/>
       <c r="G12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -5823,1039 +5792,1062 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D65D27-CBA3-A04B-A10C-1BF81BF99E43}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="140"/>
-    <col min="2" max="2" width="38" style="149" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="150" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" style="150" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="150" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="134"/>
+    <col min="2" max="2" width="38" style="143" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="144" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="144" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="144" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="144" customWidth="1"/>
     <col min="7" max="7" width="14" style="98" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" style="150" customWidth="1"/>
-    <col min="10" max="10" width="11" style="150" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="140"/>
-    <col min="12" max="16384" width="10.83203125" style="147"/>
+    <col min="8" max="8" width="12.6640625" style="144" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="144" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" style="144" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="134"/>
+    <col min="12" max="16384" width="10.83203125" style="141"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" s="146"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
       <c r="G1" s="96"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-    </row>
-    <row r="2" spans="1:11" s="164" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="160"/>
-      <c r="B2" s="161"/>
-      <c r="C2" s="162" t="s">
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+    </row>
+    <row r="2" spans="1:11" s="156" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="154"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="163" t="s">
         <v>201</v>
       </c>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="163" t="s">
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="164" t="s">
         <v>202</v>
       </c>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="160"/>
+      <c r="H2" s="164"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="136"/>
-      <c r="C3" s="137" t="s">
+      <c r="B3" s="130"/>
+      <c r="C3" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="137" t="s">
+      <c r="D3" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="137" t="s">
+      <c r="E3" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="137" t="s">
+      <c r="F3" s="131" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="137" t="s">
+      <c r="H3" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="137" t="s">
+      <c r="I3" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="137" t="s">
+      <c r="J3" s="131" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="139" t="s">
-        <v>590</v>
-      </c>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
+      <c r="B4" s="133" t="s">
+        <v>589</v>
+      </c>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
       <c r="G4" s="97"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
+      <c r="J4" s="132"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="146" t="s">
+      <c r="B5" s="140" t="s">
         <v>376</v>
       </c>
-      <c r="C5" s="135" t="s">
+      <c r="C5" s="129" t="s">
         <v>327</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="129" t="s">
         <v>491</v>
       </c>
-      <c r="E5" s="135" t="s">
+      <c r="E5" s="129" t="s">
         <v>492</v>
       </c>
-      <c r="F5" s="135" t="s">
+      <c r="F5" s="129" t="s">
         <v>493</v>
       </c>
       <c r="G5" s="96" t="s">
         <v>494</v>
       </c>
-      <c r="H5" s="135" t="s">
+      <c r="H5" s="129" t="s">
         <v>495</v>
       </c>
-      <c r="I5" s="135" t="s">
+      <c r="I5" s="129" t="s">
         <v>496</v>
       </c>
-      <c r="J5" s="135" t="s">
+      <c r="J5" s="129" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="146" t="s">
+      <c r="B6" s="140" t="s">
         <v>377</v>
       </c>
-      <c r="C6" s="135" t="s">
+      <c r="C6" s="129" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="135" t="s">
+      <c r="D6" s="129" t="s">
         <v>488</v>
       </c>
-      <c r="E6" s="135" t="s">
+      <c r="E6" s="129" t="s">
         <v>498</v>
       </c>
-      <c r="F6" s="135" t="s">
+      <c r="F6" s="129" t="s">
         <v>499</v>
       </c>
       <c r="G6" s="96" t="s">
         <v>232</v>
       </c>
-      <c r="H6" s="135" t="s">
+      <c r="H6" s="129" t="s">
         <v>500</v>
       </c>
-      <c r="I6" s="135" t="s">
+      <c r="I6" s="129" t="s">
         <v>501</v>
       </c>
-      <c r="J6" s="135" t="s">
+      <c r="J6" s="129" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="146" t="s">
+      <c r="B7" s="145" t="s">
         <v>378</v>
       </c>
-      <c r="C7" s="135" t="s">
+      <c r="C7" s="129" t="s">
         <v>473</v>
       </c>
-      <c r="D7" s="135" t="s">
+      <c r="D7" s="129" t="s">
         <v>505</v>
       </c>
-      <c r="E7" s="135" t="s">
+      <c r="E7" s="129" t="s">
         <v>506</v>
       </c>
-      <c r="F7" s="135" t="s">
+      <c r="F7" s="129" t="s">
         <v>487</v>
       </c>
-      <c r="G7" s="159" t="s">
+      <c r="G7" s="153" t="s">
+        <v>585</v>
+      </c>
+      <c r="H7" s="146" t="s">
+        <v>507</v>
+      </c>
+      <c r="I7" s="147" t="s">
+        <v>508</v>
+      </c>
+      <c r="J7" s="146" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="145" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" s="152" t="s">
+        <v>348</v>
+      </c>
+      <c r="D8" s="146" t="s">
+        <v>486</v>
+      </c>
+      <c r="E8" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="146" t="s">
+        <v>487</v>
+      </c>
+      <c r="G8" s="96"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="140" t="s">
+        <v>381</v>
+      </c>
+      <c r="C9" s="129" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="129" t="s">
+        <v>488</v>
+      </c>
+      <c r="E9" s="129" t="s">
+        <v>257</v>
+      </c>
+      <c r="F9" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G9" s="96"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="129"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="140" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" s="129" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="129" t="s">
+        <v>489</v>
+      </c>
+      <c r="E10" s="129" t="s">
+        <v>490</v>
+      </c>
+      <c r="F10" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G10" s="96"/>
+      <c r="H10" s="129"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="140" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" s="129" t="s">
+        <v>503</v>
+      </c>
+      <c r="D11" s="129" t="s">
+        <v>504</v>
+      </c>
+      <c r="E11" s="129" t="s">
+        <v>190</v>
+      </c>
+      <c r="F11" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G11" s="96"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="129"/>
+      <c r="J11" s="129"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="158" t="s">
+        <v>574</v>
+      </c>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="105" t="s">
+        <v>588</v>
+      </c>
+      <c r="H12" s="137" t="s">
+        <v>575</v>
+      </c>
+      <c r="I12" s="138" t="s">
+        <v>576</v>
+      </c>
+      <c r="J12" s="137" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="133" t="s">
+        <v>358</v>
+      </c>
+      <c r="C13" s="129"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="142"/>
+      <c r="J13" s="129"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="140" t="s">
+        <v>357</v>
+      </c>
+      <c r="C14" s="129" t="s">
+        <v>517</v>
+      </c>
+      <c r="D14" s="129" t="s">
+        <v>518</v>
+      </c>
+      <c r="E14" s="129" t="s">
+        <v>519</v>
+      </c>
+      <c r="F14" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G14" s="96" t="s">
         <v>586</v>
       </c>
-      <c r="H7" s="152" t="s">
-        <v>507</v>
-      </c>
-      <c r="I7" s="153" t="s">
-        <v>508</v>
-      </c>
-      <c r="J7" s="152" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="151" t="s">
-        <v>379</v>
-      </c>
-      <c r="C8" s="158" t="s">
-        <v>348</v>
-      </c>
-      <c r="D8" s="152" t="s">
-        <v>486</v>
-      </c>
-      <c r="E8" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="152" t="s">
-        <v>487</v>
-      </c>
-      <c r="G8" s="96"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="135"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="146" t="s">
-        <v>381</v>
-      </c>
-      <c r="C9" s="135" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="135" t="s">
-        <v>488</v>
-      </c>
-      <c r="E9" s="135" t="s">
-        <v>257</v>
-      </c>
-      <c r="F9" s="135" t="s">
-        <v>487</v>
-      </c>
-      <c r="G9" s="96"/>
-      <c r="H9" s="135"/>
-      <c r="I9" s="135"/>
-      <c r="J9" s="135"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="146" t="s">
-        <v>382</v>
-      </c>
-      <c r="C10" s="135" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="135" t="s">
-        <v>489</v>
-      </c>
-      <c r="E10" s="135" t="s">
-        <v>490</v>
-      </c>
-      <c r="F10" s="135" t="s">
-        <v>487</v>
-      </c>
-      <c r="G10" s="96"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="135"/>
-      <c r="J10" s="135"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="146" t="s">
-        <v>383</v>
-      </c>
-      <c r="C11" s="135" t="s">
-        <v>503</v>
-      </c>
-      <c r="D11" s="135" t="s">
-        <v>504</v>
-      </c>
-      <c r="E11" s="135" t="s">
-        <v>190</v>
-      </c>
-      <c r="F11" s="135" t="s">
-        <v>487</v>
-      </c>
-      <c r="G11" s="96"/>
-      <c r="H11" s="135"/>
-      <c r="I11" s="135"/>
-      <c r="J11" s="135"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="141" t="s">
-        <v>575</v>
-      </c>
-      <c r="C12" s="142"/>
-      <c r="D12" s="142"/>
-      <c r="E12" s="142"/>
-      <c r="F12" s="142"/>
-      <c r="G12" s="105" t="s">
-        <v>589</v>
-      </c>
-      <c r="H12" s="143" t="s">
-        <v>576</v>
-      </c>
-      <c r="I12" s="144" t="s">
-        <v>577</v>
-      </c>
-      <c r="J12" s="143" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="139" t="s">
-        <v>358</v>
-      </c>
-      <c r="C13" s="135"/>
-      <c r="D13" s="135"/>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="135"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="135"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="146" t="s">
-        <v>357</v>
-      </c>
-      <c r="C14" s="135" t="s">
-        <v>517</v>
-      </c>
-      <c r="D14" s="135" t="s">
-        <v>518</v>
-      </c>
-      <c r="E14" s="135" t="s">
-        <v>519</v>
-      </c>
-      <c r="F14" s="135" t="s">
-        <v>487</v>
-      </c>
-      <c r="G14" s="96" t="s">
-        <v>587</v>
-      </c>
-      <c r="H14" s="135" t="s">
+      <c r="H14" s="129" t="s">
         <v>520</v>
       </c>
-      <c r="I14" s="135" t="s">
+      <c r="I14" s="129" t="s">
         <v>521</v>
       </c>
-      <c r="J14" s="135" t="s">
+      <c r="J14" s="129" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="146" t="s">
+      <c r="B15" s="140" t="s">
         <v>359</v>
       </c>
-      <c r="C15" s="135" t="s">
+      <c r="C15" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="135" t="s">
+      <c r="D15" s="129" t="s">
         <v>523</v>
       </c>
-      <c r="E15" s="135" t="s">
+      <c r="E15" s="129" t="s">
         <v>524</v>
       </c>
-      <c r="F15" s="135" t="s">
+      <c r="F15" s="129" t="s">
         <v>525</v>
       </c>
       <c r="G15" s="96" t="s">
-        <v>586</v>
-      </c>
-      <c r="H15" s="135" t="s">
+        <v>585</v>
+      </c>
+      <c r="H15" s="129" t="s">
         <v>526</v>
       </c>
-      <c r="I15" s="135" t="s">
+      <c r="I15" s="129" t="s">
         <v>527</v>
       </c>
-      <c r="J15" s="135" t="s">
+      <c r="J15" s="129" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="140" t="s">
         <v>360</v>
       </c>
-      <c r="C16" s="135" t="s">
+      <c r="C16" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="135" t="s">
+      <c r="D16" s="129" t="s">
         <v>531</v>
       </c>
-      <c r="E16" s="135" t="s">
+      <c r="E16" s="129" t="s">
         <v>532</v>
       </c>
-      <c r="F16" s="135" t="s">
+      <c r="F16" s="129" t="s">
         <v>487</v>
       </c>
       <c r="G16" s="96" t="s">
         <v>494</v>
       </c>
-      <c r="H16" s="135" t="s">
+      <c r="H16" s="129" t="s">
         <v>533</v>
       </c>
-      <c r="I16" s="135" t="s">
+      <c r="I16" s="129" t="s">
         <v>534</v>
       </c>
-      <c r="J16" s="135" t="s">
+      <c r="J16" s="129" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="145" t="s">
         <v>361</v>
       </c>
-      <c r="C17" s="158" t="s">
+      <c r="C17" s="152" t="s">
         <v>310</v>
       </c>
-      <c r="D17" s="152" t="s">
+      <c r="D17" s="146" t="s">
         <v>510</v>
       </c>
-      <c r="E17" s="153" t="s">
+      <c r="E17" s="147" t="s">
         <v>511</v>
       </c>
-      <c r="F17" s="152" t="s">
+      <c r="F17" s="146" t="s">
         <v>487</v>
       </c>
       <c r="G17" s="96"/>
-      <c r="H17" s="135"/>
-      <c r="I17" s="135"/>
-      <c r="J17" s="135"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="129"/>
+      <c r="J17" s="129"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="140" t="s">
         <v>362</v>
       </c>
-      <c r="C18" s="135" t="s">
+      <c r="C18" s="129" t="s">
         <v>512</v>
       </c>
-      <c r="D18" s="135" t="s">
+      <c r="D18" s="129" t="s">
         <v>513</v>
       </c>
-      <c r="E18" s="135" t="s">
+      <c r="E18" s="129" t="s">
         <v>514</v>
       </c>
-      <c r="F18" s="135" t="s">
+      <c r="F18" s="129" t="s">
         <v>487</v>
       </c>
       <c r="G18" s="96"/>
-      <c r="H18" s="135"/>
-      <c r="I18" s="135"/>
-      <c r="J18" s="135"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="129"/>
+      <c r="J18" s="129"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="146" t="s">
+      <c r="B19" s="140" t="s">
         <v>363</v>
       </c>
-      <c r="C19" s="135" t="s">
+      <c r="C19" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="135" t="s">
+      <c r="D19" s="129" t="s">
         <v>515</v>
       </c>
-      <c r="E19" s="135" t="s">
+      <c r="E19" s="129" t="s">
         <v>516</v>
       </c>
-      <c r="F19" s="135" t="s">
+      <c r="F19" s="129" t="s">
         <v>487</v>
       </c>
       <c r="G19" s="96"/>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
-      <c r="J19" s="135"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="129"/>
+      <c r="J19" s="129"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="146" t="s">
+      <c r="B20" s="140" t="s">
         <v>364</v>
       </c>
-      <c r="C20" s="135" t="s">
+      <c r="C20" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="135" t="s">
+      <c r="D20" s="129" t="s">
         <v>529</v>
       </c>
-      <c r="E20" s="135" t="s">
+      <c r="E20" s="129" t="s">
         <v>530</v>
       </c>
-      <c r="F20" s="135" t="s">
+      <c r="F20" s="129" t="s">
         <v>487</v>
       </c>
       <c r="G20" s="96"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="135"/>
-      <c r="J20" s="135"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
+      <c r="J20" s="129"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="135" t="s">
         <v>365</v>
       </c>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142"/>
-      <c r="E21" s="142"/>
-      <c r="F21" s="142"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="136"/>
       <c r="G21" s="93" t="s">
+        <v>577</v>
+      </c>
+      <c r="H21" s="136" t="s">
         <v>578</v>
       </c>
-      <c r="H21" s="142" t="s">
+      <c r="I21" s="136" t="s">
         <v>579</v>
       </c>
-      <c r="I21" s="142" t="s">
+      <c r="J21" s="136" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="133" t="s">
+        <v>366</v>
+      </c>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="129"/>
+      <c r="I22" s="129"/>
+      <c r="J22" s="129"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="140" t="s">
+        <v>367</v>
+      </c>
+      <c r="C23" s="129" t="s">
+        <v>221</v>
+      </c>
+      <c r="D23" s="129" t="s">
+        <v>542</v>
+      </c>
+      <c r="E23" s="129" t="s">
+        <v>521</v>
+      </c>
+      <c r="F23" s="129" t="s">
+        <v>543</v>
+      </c>
+      <c r="G23" s="96" t="s">
+        <v>544</v>
+      </c>
+      <c r="H23" s="129" t="s">
+        <v>545</v>
+      </c>
+      <c r="I23" s="129" t="s">
+        <v>546</v>
+      </c>
+      <c r="J23" s="129" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="145" t="s">
+        <v>368</v>
+      </c>
+      <c r="C24" s="152" t="s">
+        <v>292</v>
+      </c>
+      <c r="D24" s="146" t="s">
+        <v>548</v>
+      </c>
+      <c r="E24" s="147" t="s">
+        <v>511</v>
+      </c>
+      <c r="F24" s="146" t="s">
+        <v>549</v>
+      </c>
+      <c r="G24" s="96" t="s">
+        <v>550</v>
+      </c>
+      <c r="H24" s="129" t="s">
+        <v>551</v>
+      </c>
+      <c r="I24" s="129" t="s">
+        <v>552</v>
+      </c>
+      <c r="J24" s="129" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="140" t="s">
+        <v>369</v>
+      </c>
+      <c r="C25" s="129" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="129" t="s">
+        <v>556</v>
+      </c>
+      <c r="E25" s="129" t="s">
+        <v>557</v>
+      </c>
+      <c r="F25" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G25" s="96" t="s">
+        <v>558</v>
+      </c>
+      <c r="H25" s="129" t="s">
+        <v>559</v>
+      </c>
+      <c r="I25" s="129" t="s">
+        <v>560</v>
+      </c>
+      <c r="J25" s="129" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="145" t="s">
+        <v>370</v>
+      </c>
+      <c r="C26" s="152" t="s">
+        <v>535</v>
+      </c>
+      <c r="D26" s="146" t="s">
+        <v>536</v>
+      </c>
+      <c r="E26" s="147" t="s">
+        <v>537</v>
+      </c>
+      <c r="F26" s="146" t="s">
+        <v>487</v>
+      </c>
+      <c r="G26" s="96"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="140" t="s">
+        <v>372</v>
+      </c>
+      <c r="C27" s="129" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="E27" s="129" t="s">
+        <v>539</v>
+      </c>
+      <c r="F27" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G27" s="96"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="129"/>
+      <c r="J27" s="129"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="140" t="s">
+        <v>373</v>
+      </c>
+      <c r="C28" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="129" t="s">
+        <v>540</v>
+      </c>
+      <c r="E28" s="129" t="s">
+        <v>541</v>
+      </c>
+      <c r="F28" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G28" s="96"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
+      <c r="J28" s="129"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="140" t="s">
+        <v>374</v>
+      </c>
+      <c r="C29" s="129" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="129" t="s">
+        <v>554</v>
+      </c>
+      <c r="E29" s="129" t="s">
+        <v>555</v>
+      </c>
+      <c r="F29" s="129" t="s">
+        <v>487</v>
+      </c>
+      <c r="G29" s="96"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="129"/>
+      <c r="J29" s="129"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="158" t="s">
+        <v>371</v>
+      </c>
+      <c r="C30" s="136"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="105" t="s">
+        <v>587</v>
+      </c>
+      <c r="H30" s="137" t="s">
         <v>580</v>
       </c>
-      <c r="J21" s="142" t="s">
+      <c r="I30" s="138" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="137" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="139" t="s">
-        <v>366</v>
-      </c>
-      <c r="C22" s="135"/>
-      <c r="D22" s="135"/>
-      <c r="E22" s="135"/>
-      <c r="F22" s="135"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="135"/>
-      <c r="I22" s="135"/>
-      <c r="J22" s="135"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="146" t="s">
-        <v>367</v>
-      </c>
-      <c r="C23" s="135" t="s">
-        <v>221</v>
-      </c>
-      <c r="D23" s="135" t="s">
-        <v>543</v>
-      </c>
-      <c r="E23" s="135" t="s">
-        <v>521</v>
-      </c>
-      <c r="F23" s="135" t="s">
-        <v>544</v>
-      </c>
-      <c r="G23" s="96" t="s">
-        <v>545</v>
-      </c>
-      <c r="H23" s="135" t="s">
-        <v>546</v>
-      </c>
-      <c r="I23" s="135" t="s">
-        <v>547</v>
-      </c>
-      <c r="J23" s="135" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="151" t="s">
-        <v>368</v>
-      </c>
-      <c r="C24" s="158" t="s">
-        <v>292</v>
-      </c>
-      <c r="D24" s="152" t="s">
-        <v>549</v>
-      </c>
-      <c r="E24" s="153" t="s">
-        <v>511</v>
-      </c>
-      <c r="F24" s="152" t="s">
-        <v>550</v>
-      </c>
-      <c r="G24" s="96" t="s">
-        <v>551</v>
-      </c>
-      <c r="H24" s="135" t="s">
-        <v>552</v>
-      </c>
-      <c r="I24" s="135" t="s">
-        <v>553</v>
-      </c>
-      <c r="J24" s="135" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="146" t="s">
-        <v>369</v>
-      </c>
-      <c r="C25" s="135" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" s="135" t="s">
-        <v>557</v>
-      </c>
-      <c r="E25" s="135" t="s">
-        <v>558</v>
-      </c>
-      <c r="F25" s="135" t="s">
+    <row r="31" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="133" t="s">
+        <v>384</v>
+      </c>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="129"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="96"/>
+      <c r="H31" s="129"/>
+      <c r="I31" s="129"/>
+      <c r="J31" s="129"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="145" t="s">
+        <v>385</v>
+      </c>
+      <c r="C32" s="148" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="146" t="s">
+        <v>564</v>
+      </c>
+      <c r="E32" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="146" t="s">
+        <v>565</v>
+      </c>
+      <c r="G32" s="149" t="s">
+        <v>188</v>
+      </c>
+      <c r="H32" s="146" t="s">
+        <v>566</v>
+      </c>
+      <c r="I32" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="146" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="145" t="s">
+        <v>386</v>
+      </c>
+      <c r="C33" s="148" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="146" t="s">
+        <v>564</v>
+      </c>
+      <c r="E33" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="146" t="s">
+        <v>568</v>
+      </c>
+      <c r="G33" s="149" t="s">
+        <v>569</v>
+      </c>
+      <c r="H33" s="146" t="s">
+        <v>570</v>
+      </c>
+      <c r="I33" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="146" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="145" t="s">
+        <v>387</v>
+      </c>
+      <c r="C34" s="148" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="146" t="s">
+        <v>572</v>
+      </c>
+      <c r="E34" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="146" t="s">
         <v>487</v>
       </c>
-      <c r="G25" s="96" t="s">
-        <v>559</v>
-      </c>
-      <c r="H25" s="135" t="s">
-        <v>560</v>
-      </c>
-      <c r="I25" s="135" t="s">
+      <c r="G34" s="149" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="146" t="s">
+        <v>573</v>
+      </c>
+      <c r="I34" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="146" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="145" t="s">
+        <v>388</v>
+      </c>
+      <c r="C35" s="148" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="146" t="s">
         <v>561</v>
       </c>
-      <c r="J25" s="135" t="s">
+      <c r="E35" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="146" t="s">
+        <v>487</v>
+      </c>
+      <c r="G35" s="150"/>
+      <c r="H35" s="129"/>
+      <c r="I35" s="129"/>
+      <c r="J35" s="129"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="145" t="s">
+        <v>390</v>
+      </c>
+      <c r="C36" s="149" t="s">
+        <v>478</v>
+      </c>
+      <c r="D36" s="146" t="s">
+        <v>562</v>
+      </c>
+      <c r="E36" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="146" t="s">
+        <v>487</v>
+      </c>
+      <c r="G36" s="150"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
+      <c r="J36" s="129"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" s="145" t="s">
+        <v>391</v>
+      </c>
+      <c r="C37" s="148" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" s="146" t="s">
+        <v>563</v>
+      </c>
+      <c r="E37" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="146" t="s">
+        <v>487</v>
+      </c>
+      <c r="G37" s="150"/>
+      <c r="H37" s="129"/>
+      <c r="I37" s="129"/>
+      <c r="J37" s="129"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="145" t="s">
+        <v>392</v>
+      </c>
+      <c r="C38" s="148" t="s">
+        <v>512</v>
+      </c>
+      <c r="D38" s="146" t="s">
+        <v>571</v>
+      </c>
+      <c r="E38" s="147" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="146" t="s">
+        <v>487</v>
+      </c>
+      <c r="G38" s="150"/>
+      <c r="H38" s="129"/>
+      <c r="I38" s="129"/>
+      <c r="J38" s="129"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="158" t="s">
+        <v>389</v>
+      </c>
+      <c r="C39" s="136"/>
+      <c r="D39" s="136"/>
+      <c r="E39" s="136"/>
+      <c r="F39" s="136"/>
+      <c r="G39" s="151" t="s">
+        <v>253</v>
+      </c>
+      <c r="H39" s="137" t="s">
+        <v>581</v>
+      </c>
+      <c r="I39" s="138" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="137" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="151" t="s">
-        <v>370</v>
-      </c>
-      <c r="C26" s="158" t="s">
-        <v>535</v>
-      </c>
-      <c r="D26" s="152" t="s">
-        <v>536</v>
-      </c>
-      <c r="E26" s="153" t="s">
-        <v>537</v>
-      </c>
-      <c r="F26" s="152" t="s">
-        <v>487</v>
-      </c>
-      <c r="G26" s="96"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
-      <c r="J26" s="135"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="146" t="s">
-        <v>372</v>
-      </c>
-      <c r="C27" s="135" t="s">
-        <v>178</v>
-      </c>
-      <c r="D27" s="135" t="s">
-        <v>538</v>
-      </c>
-      <c r="E27" s="135" t="s">
-        <v>539</v>
-      </c>
-      <c r="F27" s="135" t="s">
-        <v>487</v>
-      </c>
-      <c r="G27" s="96"/>
-      <c r="H27" s="135"/>
-      <c r="I27" s="135"/>
-      <c r="J27" s="135"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="146" t="s">
-        <v>373</v>
-      </c>
-      <c r="C28" s="135" t="s">
-        <v>540</v>
-      </c>
-      <c r="D28" s="135" t="s">
-        <v>541</v>
-      </c>
-      <c r="E28" s="135" t="s">
-        <v>542</v>
-      </c>
-      <c r="F28" s="135" t="s">
-        <v>487</v>
-      </c>
-      <c r="G28" s="96"/>
-      <c r="H28" s="135"/>
-      <c r="I28" s="135"/>
-      <c r="J28" s="135"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="146" t="s">
-        <v>374</v>
-      </c>
-      <c r="C29" s="135" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="135" t="s">
-        <v>555</v>
-      </c>
-      <c r="E29" s="135" t="s">
+    <row r="40" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="139" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="129"/>
+      <c r="D40" s="129"/>
+      <c r="E40" s="129"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="129"/>
+      <c r="I40" s="129"/>
+      <c r="J40" s="129"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="140" t="s">
+        <v>353</v>
+      </c>
+      <c r="C41" s="129" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="129"/>
+      <c r="G41" s="96" t="s">
+        <v>582</v>
+      </c>
+      <c r="H41" s="129"/>
+      <c r="I41" s="129"/>
+      <c r="J41" s="129"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="140" t="s">
+        <v>354</v>
+      </c>
+      <c r="C42" s="129" t="s">
+        <v>313</v>
+      </c>
+      <c r="D42" s="129"/>
+      <c r="E42" s="129"/>
+      <c r="F42" s="129"/>
+      <c r="G42" s="96" t="s">
+        <v>590</v>
+      </c>
+      <c r="H42" s="129"/>
+      <c r="I42" s="129"/>
+      <c r="J42" s="129"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="82" t="s">
+        <v>395</v>
+      </c>
+      <c r="C43" s="157">
+        <v>490</v>
+      </c>
+      <c r="D43" s="129"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="96" t="s">
+        <v>592</v>
+      </c>
+      <c r="H43" s="129"/>
+      <c r="I43" s="129"/>
+      <c r="J43" s="129"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="82" t="s">
+        <v>396</v>
+      </c>
+      <c r="C44" s="157">
+        <v>28</v>
+      </c>
+      <c r="D44" s="129"/>
+      <c r="E44" s="129"/>
+      <c r="F44" s="129"/>
+      <c r="G44" s="96" t="s">
+        <v>399</v>
+      </c>
+      <c r="H44" s="129"/>
+      <c r="I44" s="129"/>
+      <c r="J44" s="129"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="140" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="157">
         <v>556</v>
       </c>
-      <c r="F29" s="135" t="s">
-        <v>487</v>
-      </c>
-      <c r="G29" s="96"/>
-      <c r="H29" s="135"/>
-      <c r="I29" s="135"/>
-      <c r="J29" s="135"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="141" t="s">
-        <v>371</v>
-      </c>
-      <c r="C30" s="142"/>
-      <c r="D30" s="142"/>
-      <c r="E30" s="142"/>
-      <c r="F30" s="142"/>
-      <c r="G30" s="105" t="s">
-        <v>588</v>
-      </c>
-      <c r="H30" s="143" t="s">
-        <v>581</v>
-      </c>
-      <c r="I30" s="144" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" s="143" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="139" t="s">
-        <v>384</v>
-      </c>
-      <c r="C31" s="135"/>
-      <c r="D31" s="135"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="135"/>
-      <c r="I31" s="135"/>
-      <c r="J31" s="135"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="151" t="s">
-        <v>385</v>
-      </c>
-      <c r="C32" s="154" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" s="152" t="s">
-        <v>565</v>
-      </c>
-      <c r="E32" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="152" t="s">
-        <v>566</v>
-      </c>
-      <c r="G32" s="155" t="s">
-        <v>188</v>
-      </c>
-      <c r="H32" s="152" t="s">
-        <v>567</v>
-      </c>
-      <c r="I32" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="152" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="151" t="s">
-        <v>386</v>
-      </c>
-      <c r="C33" s="154" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="152" t="s">
-        <v>565</v>
-      </c>
-      <c r="E33" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="152" t="s">
-        <v>569</v>
-      </c>
-      <c r="G33" s="155" t="s">
-        <v>570</v>
-      </c>
-      <c r="H33" s="152" t="s">
-        <v>571</v>
-      </c>
-      <c r="I33" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="152" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="151" t="s">
-        <v>387</v>
-      </c>
-      <c r="C34" s="154" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="152" t="s">
-        <v>573</v>
-      </c>
-      <c r="E34" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="152" t="s">
-        <v>487</v>
-      </c>
-      <c r="G34" s="155" t="s">
-        <v>111</v>
-      </c>
-      <c r="H34" s="152" t="s">
-        <v>574</v>
-      </c>
-      <c r="I34" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="J34" s="152" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="151" t="s">
-        <v>388</v>
-      </c>
-      <c r="C35" s="154" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="152" t="s">
-        <v>562</v>
-      </c>
-      <c r="E35" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="152" t="s">
-        <v>487</v>
-      </c>
-      <c r="G35" s="156"/>
-      <c r="H35" s="135"/>
-      <c r="I35" s="135"/>
-      <c r="J35" s="135"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="151" t="s">
-        <v>390</v>
-      </c>
-      <c r="C36" s="154" t="s">
-        <v>540</v>
-      </c>
-      <c r="D36" s="152" t="s">
-        <v>563</v>
-      </c>
-      <c r="E36" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="152" t="s">
-        <v>487</v>
-      </c>
-      <c r="G36" s="156"/>
-      <c r="H36" s="135"/>
-      <c r="I36" s="135"/>
-      <c r="J36" s="135"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="151" t="s">
-        <v>391</v>
-      </c>
-      <c r="C37" s="154" t="s">
-        <v>195</v>
-      </c>
-      <c r="D37" s="152" t="s">
-        <v>564</v>
-      </c>
-      <c r="E37" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="152" t="s">
-        <v>487</v>
-      </c>
-      <c r="G37" s="156"/>
-      <c r="H37" s="135"/>
-      <c r="I37" s="135"/>
-      <c r="J37" s="135"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="151" t="s">
-        <v>392</v>
-      </c>
-      <c r="C38" s="154" t="s">
-        <v>512</v>
-      </c>
-      <c r="D38" s="152" t="s">
-        <v>572</v>
-      </c>
-      <c r="E38" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="152" t="s">
-        <v>487</v>
-      </c>
-      <c r="G38" s="156"/>
-      <c r="H38" s="135"/>
-      <c r="I38" s="135"/>
-      <c r="J38" s="135"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="141" t="s">
-        <v>389</v>
-      </c>
-      <c r="C39" s="142"/>
-      <c r="D39" s="142"/>
-      <c r="E39" s="142"/>
-      <c r="F39" s="142"/>
-      <c r="G39" s="157" t="s">
-        <v>253</v>
-      </c>
-      <c r="H39" s="143" t="s">
-        <v>582</v>
-      </c>
-      <c r="I39" s="144" t="s">
-        <v>11</v>
-      </c>
-      <c r="J39" s="143" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="145" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="135"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="135"/>
-      <c r="G40" s="96"/>
-      <c r="H40" s="135"/>
-      <c r="I40" s="135"/>
-      <c r="J40" s="135"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="146" t="s">
-        <v>353</v>
-      </c>
-      <c r="C41" s="135" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="135"/>
-      <c r="E41" s="135"/>
-      <c r="F41" s="135"/>
-      <c r="G41" s="96" t="s">
+      <c r="D45" s="129"/>
+      <c r="E45" s="129"/>
+      <c r="F45" s="129"/>
+      <c r="G45" s="96">
+        <v>76</v>
+      </c>
+      <c r="H45" s="129"/>
+      <c r="I45" s="129"/>
+      <c r="J45" s="129"/>
+    </row>
+    <row r="46" spans="2:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="B46" s="135" t="s">
+        <v>591</v>
+      </c>
+      <c r="C46" s="136" t="s">
         <v>583</v>
       </c>
-      <c r="H41" s="135"/>
-      <c r="I41" s="135"/>
-      <c r="J41" s="135"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="146" t="s">
-        <v>354</v>
-      </c>
-      <c r="C42" s="135" t="s">
-        <v>313</v>
-      </c>
-      <c r="D42" s="135"/>
-      <c r="E42" s="135"/>
-      <c r="F42" s="135"/>
-      <c r="G42" s="96" t="s">
-        <v>591</v>
-      </c>
-      <c r="H42" s="135"/>
-      <c r="I42" s="135"/>
-      <c r="J42" s="135"/>
-    </row>
-    <row r="43" spans="2:10" ht="20" x14ac:dyDescent="0.2">
-      <c r="B43" s="146" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="135" t="s">
-        <v>592</v>
-      </c>
-      <c r="D43" s="135"/>
-      <c r="E43" s="135"/>
-      <c r="F43" s="135"/>
-      <c r="G43" s="96" t="s">
-        <v>593</v>
-      </c>
-      <c r="H43" s="135"/>
-      <c r="I43" s="135"/>
-      <c r="J43" s="135"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B44" s="146" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="135">
-        <v>556</v>
-      </c>
-      <c r="D44" s="135"/>
-      <c r="E44" s="135"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="96">
-        <v>76</v>
-      </c>
-      <c r="H44" s="135"/>
-      <c r="I44" s="135"/>
-      <c r="J44" s="135"/>
-    </row>
-    <row r="45" spans="2:10" ht="21" x14ac:dyDescent="0.2">
-      <c r="B45" s="141" t="s">
-        <v>594</v>
-      </c>
-      <c r="C45" s="142" t="s">
+      <c r="D46" s="136"/>
+      <c r="E46" s="136"/>
+      <c r="F46" s="136"/>
+      <c r="G46" s="93" t="s">
         <v>584</v>
       </c>
-      <c r="D45" s="142"/>
-      <c r="E45" s="142"/>
-      <c r="F45" s="142"/>
-      <c r="G45" s="93" t="s">
-        <v>585</v>
-      </c>
-      <c r="H45" s="142"/>
-      <c r="I45" s="142"/>
-      <c r="J45" s="142"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="146"/>
-      <c r="C46" s="135"/>
-      <c r="D46" s="135"/>
-      <c r="E46" s="135"/>
-      <c r="F46" s="135"/>
-      <c r="G46" s="96"/>
-      <c r="H46" s="135"/>
-      <c r="I46" s="135"/>
-      <c r="J46" s="135"/>
+      <c r="H46" s="136"/>
+      <c r="I46" s="136"/>
+      <c r="J46" s="136"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="146"/>
-      <c r="C47" s="135"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="135"/>
-      <c r="F47" s="135"/>
+      <c r="B47" s="140"/>
+      <c r="C47" s="129"/>
+      <c r="D47" s="129"/>
+      <c r="E47" s="129"/>
+      <c r="F47" s="129"/>
       <c r="G47" s="96"/>
-      <c r="H47" s="135"/>
-      <c r="I47" s="135"/>
-      <c r="J47" s="135"/>
+      <c r="H47" s="129"/>
+      <c r="I47" s="129"/>
+      <c r="J47" s="129"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="146"/>
-      <c r="C48" s="135"/>
-      <c r="D48" s="135"/>
-      <c r="E48" s="135"/>
-      <c r="F48" s="135"/>
+      <c r="B48" s="140"/>
+      <c r="C48" s="129"/>
+      <c r="D48" s="129"/>
+      <c r="E48" s="129"/>
+      <c r="F48" s="129"/>
       <c r="G48" s="96"/>
-      <c r="H48" s="135"/>
-      <c r="I48" s="135"/>
-      <c r="J48" s="135"/>
-    </row>
-    <row r="52" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H48" s="129"/>
+      <c r="I48" s="129"/>
+      <c r="J48" s="129"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="140"/>
+      <c r="C49" s="129"/>
+      <c r="D49" s="129"/>
+      <c r="E49" s="129"/>
+      <c r="F49" s="129"/>
+      <c r="G49" s="96"/>
+      <c r="H49" s="129"/>
+      <c r="I49" s="129"/>
+      <c r="J49" s="129"/>
+    </row>
+    <row r="53" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G43:G44" numberStoredAsText="1"/>
+    <ignoredError sqref="G30 G7 G12 G14:G15" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -6863,8 +6855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F98581C-D690-F849-931B-53E74322DAFE}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L43"/>
+    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -6902,20 +6894,20 @@
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="81"/>
       <c r="B2" s="82"/>
-      <c r="C2" s="133" t="s">
+      <c r="C2" s="165" t="s">
         <v>201</v>
       </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
       <c r="G2" s="96"/>
-      <c r="H2" s="134" t="s">
+      <c r="H2" s="166" t="s">
         <v>202</v>
       </c>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
       <c r="M2" s="81"/>
     </row>
     <row r="3" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
-beta offet estimate + 1-beta pvalue
</commit_message>
<xml_diff>
--- a/results/Models/Table_models_MEP.xlsx
+++ b/results/Models/Table_models_MEP.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beckeant/Library/CloudStorage/OneDrive-UniversityofHelsinki/ABS_Postdoc/Helsinki/Work/Arctic_Flowering/Zackenberg_Flowering/results/Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helsinkifi-my.sharepoint.com/personal/beckeant_ad_helsinki_fi/Documents/ABS_Postdoc/Helsinki/Work/Arctic_Flowering/Zackenberg_Flowering/results/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D963F0-84F9-6D45-8769-7E8B137B3587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{576608AB-0FCB-0748-BB3E-3D70AA25B7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80A1118C-3C9D-C645-8642-F27FBB1FE90F}"/>
   <bookViews>
-    <workbookView xWindow="-5720" yWindow="-21100" windowWidth="18000" windowHeight="21100" activeTab="3" xr2:uid="{21647BD2-5D45-904F-BF0E-D57BB03BEE0E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{21647BD2-5D45-904F-BF0E-D57BB03BEE0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Study_design" sheetId="8" r:id="rId1"/>
     <sheet name="Eq1_site_mod" sheetId="11" r:id="rId2"/>
     <sheet name="Eq2_species_mods" sheetId="9" r:id="rId3"/>
     <sheet name="Eq3_offset" sheetId="16" r:id="rId4"/>
-    <sheet name="EQ3_drivers_INT_mod" sheetId="13" r:id="rId5"/>
+    <sheet name="OLD_eq3" sheetId="13" r:id="rId5"/>
     <sheet name="Clim_Seasonal_trends" sheetId="14" r:id="rId6"/>
     <sheet name="Snow_melt" sheetId="15" r:id="rId7"/>
     <sheet name="Summary" sheetId="12" r:id="rId8"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="603">
   <si>
     <t>Predictors</t>
   </si>
@@ -432,9 +432,6 @@
   </si>
   <si>
     <t>0.024</t>
-  </si>
-  <si>
-    <t>-0.14</t>
   </si>
   <si>
     <t>0.10</t>
@@ -762,9 +759,6 @@
     <t>0.199</t>
   </si>
   <si>
-    <t>-0.24</t>
-  </si>
-  <si>
     <t>0.182</t>
   </si>
   <si>
@@ -1903,9 +1897,6 @@
   </si>
   <si>
     <t>527.69</t>
-  </si>
-  <si>
-    <t>-0.39</t>
   </si>
   <si>
     <t>-0.79 – 0.01</t>
@@ -2007,12 +1998,54 @@
   <si>
     <t>54</t>
   </si>
+  <si>
+    <t>Value corrected offset : 1-(-beta)</t>
+  </si>
+  <si>
+    <t>Zack_1-beta</t>
+  </si>
+  <si>
+    <t>Zack_orig</t>
+  </si>
+  <si>
+    <t>Nuuk_orig</t>
+  </si>
+  <si>
+    <t>Nuuk_1-beta</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.997</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2250,8 +2283,15 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2279,6 +2319,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2324,7 +2376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2788,6 +2840,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="36" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="36" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="35" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="36" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4665,7 +4741,7 @@
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
       <c r="D1" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -4680,10 +4756,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="36"/>
@@ -4701,7 +4777,7 @@
     <row r="3" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="37"/>
@@ -4713,7 +4789,7 @@
       <c r="H3" s="160"/>
       <c r="I3" s="38"/>
       <c r="J3" s="160" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K3" s="160"/>
       <c r="L3" s="160"/>
@@ -4757,32 +4833,32 @@
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
       <c r="D5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="N5" s="35"/>
     </row>
@@ -4794,29 +4870,29 @@
         <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="K6" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="K6" s="31" t="s">
-        <v>125</v>
-      </c>
       <c r="L6" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6" s="31" t="s">
         <v>121</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>122</v>
       </c>
       <c r="N6" s="35"/>
     </row>
@@ -4825,17 +4901,17 @@
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
       <c r="D7" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="161" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F7" s="161"/>
       <c r="G7" s="161"/>
       <c r="H7" s="161"/>
       <c r="I7" s="7"/>
       <c r="J7" s="161" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K7" s="161"/>
       <c r="L7" s="161"/>
@@ -4913,10 +4989,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -4935,7 +5011,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="63" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N3" s="63" t="s">
         <v>4</v>
@@ -4960,10 +5036,10 @@
       <c r="B5" s="61"/>
       <c r="K5" s="2"/>
       <c r="L5" s="66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M5" s="62" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N5" s="62">
         <v>7</v>
@@ -4980,7 +5056,7 @@
         <v>23</v>
       </c>
       <c r="M6" s="62" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N6" s="62">
         <v>1</v>
@@ -4994,10 +5070,10 @@
       <c r="B7" s="61"/>
       <c r="K7" s="2"/>
       <c r="L7" s="66" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M7" s="62" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N7" s="62">
         <v>6</v>
@@ -5022,10 +5098,10 @@
       <c r="B9" s="61"/>
       <c r="K9" s="2"/>
       <c r="L9" s="66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M9" s="62" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N9" s="70">
         <v>5</v>
@@ -5042,7 +5118,7 @@
         <v>23</v>
       </c>
       <c r="M10" s="62" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N10" s="70">
         <v>1</v>
@@ -5054,14 +5130,14 @@
     </row>
     <row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="71" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M11" s="72" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N11" s="73">
         <v>4</v>
@@ -5130,16 +5206,16 @@
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="8" t="s">
@@ -5155,16 +5231,16 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -5174,16 +5250,16 @@
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G17" s="2"/>
     </row>
@@ -5193,16 +5269,16 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G18" s="2"/>
     </row>
@@ -5212,16 +5288,16 @@
         <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="G19" s="2"/>
     </row>
@@ -5231,16 +5307,16 @@
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G20" s="2"/>
     </row>
@@ -5250,16 +5326,16 @@
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G21" s="2"/>
     </row>
@@ -5269,16 +5345,16 @@
         <v>23</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E22" s="60" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G22" s="2"/>
     </row>
@@ -5288,16 +5364,16 @@
         <v>24</v>
       </c>
       <c r="C23" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="E23" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="E23" s="60" t="s">
-        <v>171</v>
-      </c>
       <c r="F23" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G23" s="2"/>
       <c r="K23" s="2"/>
@@ -5313,16 +5389,16 @@
         <v>25</v>
       </c>
       <c r="C24" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="31" t="s">
         <v>172</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>173</v>
       </c>
       <c r="E24" s="60" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G24" s="2"/>
       <c r="K24" s="2"/>
@@ -5338,16 +5414,16 @@
         <v>29</v>
       </c>
       <c r="C25" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="31" t="s">
         <v>174</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>175</v>
       </c>
       <c r="E25" s="60" t="s">
         <v>109</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G25" s="2"/>
       <c r="K25" s="2"/>
@@ -5358,16 +5434,16 @@
         <v>26</v>
       </c>
       <c r="C26" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="31" t="s">
         <v>174</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>175</v>
       </c>
       <c r="E26" s="60" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G26" s="2"/>
       <c r="K26" s="2"/>
@@ -5382,16 +5458,16 @@
         <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G27" s="2"/>
       <c r="K27" s="2"/>
@@ -5406,16 +5482,16 @@
         <v>28</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E28" s="60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -5436,7 +5512,7 @@
         <v>104</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -5448,7 +5524,7 @@
         <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -5461,7 +5537,7 @@
         <v>99</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -5474,7 +5550,7 @@
         <v>105</v>
       </c>
       <c r="C33" s="57" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -5792,10 +5868,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D65D27-CBA3-A04B-A10C-1BF81BF99E43}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q35" sqref="Q35:Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -5811,7 +5887,13 @@
     <col min="9" max="9" width="13.6640625" style="144" customWidth="1"/>
     <col min="10" max="10" width="9.6640625" style="144" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="134"/>
-    <col min="12" max="16384" width="10.83203125" style="141"/>
+    <col min="12" max="12" width="10.83203125" style="141"/>
+    <col min="13" max="13" width="11.83203125" style="141" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="141" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.33203125" style="141" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" style="141" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" style="141" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="141"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -5829,13 +5911,13 @@
       <c r="A2" s="154"/>
       <c r="B2" s="155"/>
       <c r="C2" s="163" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D2" s="163"/>
       <c r="E2" s="163"/>
       <c r="F2" s="163"/>
       <c r="G2" s="164" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H2" s="164"/>
       <c r="I2" s="164"/>
@@ -5871,7 +5953,7 @@
     </row>
     <row r="4" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="133" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C4" s="132"/>
       <c r="D4" s="132"/>
@@ -5884,106 +5966,106 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="140" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C5" s="129" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D5" s="129" t="s">
+        <v>489</v>
+      </c>
+      <c r="E5" s="129" t="s">
+        <v>490</v>
+      </c>
+      <c r="F5" s="129" t="s">
         <v>491</v>
       </c>
-      <c r="E5" s="129" t="s">
+      <c r="G5" s="96" t="s">
         <v>492</v>
       </c>
-      <c r="F5" s="129" t="s">
+      <c r="H5" s="129" t="s">
         <v>493</v>
       </c>
-      <c r="G5" s="96" t="s">
+      <c r="I5" s="129" t="s">
         <v>494</v>
       </c>
-      <c r="H5" s="129" t="s">
+      <c r="J5" s="129" t="s">
         <v>495</v>
-      </c>
-      <c r="I5" s="129" t="s">
-        <v>496</v>
-      </c>
-      <c r="J5" s="129" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="140" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C6" s="129" t="s">
         <v>108</v>
       </c>
       <c r="D6" s="129" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E6" s="129" t="s">
+        <v>496</v>
+      </c>
+      <c r="F6" s="129" t="s">
+        <v>497</v>
+      </c>
+      <c r="G6" s="96" t="s">
+        <v>230</v>
+      </c>
+      <c r="H6" s="129" t="s">
         <v>498</v>
       </c>
-      <c r="F6" s="129" t="s">
+      <c r="I6" s="129" t="s">
         <v>499</v>
       </c>
-      <c r="G6" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="H6" s="129" t="s">
+      <c r="J6" s="129" t="s">
         <v>500</v>
-      </c>
-      <c r="I6" s="129" t="s">
-        <v>501</v>
-      </c>
-      <c r="J6" s="129" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="145" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D7" s="129" t="s">
+        <v>503</v>
+      </c>
+      <c r="E7" s="129" t="s">
+        <v>504</v>
+      </c>
+      <c r="F7" s="129" t="s">
+        <v>485</v>
+      </c>
+      <c r="G7" s="153" t="s">
+        <v>582</v>
+      </c>
+      <c r="H7" s="146" t="s">
         <v>505</v>
       </c>
-      <c r="E7" s="129" t="s">
+      <c r="I7" s="147" t="s">
         <v>506</v>
       </c>
-      <c r="F7" s="129" t="s">
-        <v>487</v>
-      </c>
-      <c r="G7" s="153" t="s">
-        <v>585</v>
-      </c>
-      <c r="H7" s="146" t="s">
+      <c r="J7" s="146" t="s">
         <v>507</v>
-      </c>
-      <c r="I7" s="147" t="s">
-        <v>508</v>
-      </c>
-      <c r="J7" s="146" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="145" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C8" s="152" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D8" s="146" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E8" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G8" s="96"/>
       <c r="H8" s="129"/>
@@ -5992,19 +6074,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="140" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C9" s="129" t="s">
         <v>108</v>
       </c>
       <c r="D9" s="129" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E9" s="129" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F9" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G9" s="96"/>
       <c r="H9" s="129"/>
@@ -6013,19 +6095,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="140" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C10" s="129" t="s">
         <v>100</v>
       </c>
       <c r="D10" s="129" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E10" s="129" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F10" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G10" s="96"/>
       <c r="H10" s="129"/>
@@ -6034,19 +6116,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="140" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C11" s="129" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D11" s="129" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E11" s="129" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F11" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G11" s="96"/>
       <c r="H11" s="129"/>
@@ -6055,28 +6137,28 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="158" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C12" s="136"/>
       <c r="D12" s="136"/>
       <c r="E12" s="136"/>
       <c r="F12" s="136"/>
       <c r="G12" s="105" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H12" s="137" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="I12" s="138" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="J12" s="137" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="133" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C13" s="129"/>
       <c r="D13" s="129"/>
@@ -6089,199 +6171,199 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="140" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C14" s="129" t="s">
+        <v>515</v>
+      </c>
+      <c r="D14" s="129" t="s">
+        <v>516</v>
+      </c>
+      <c r="E14" s="129" t="s">
         <v>517</v>
       </c>
-      <c r="D14" s="129" t="s">
+      <c r="F14" s="129" t="s">
+        <v>485</v>
+      </c>
+      <c r="G14" s="96" t="s">
+        <v>583</v>
+      </c>
+      <c r="H14" s="129" t="s">
         <v>518</v>
       </c>
-      <c r="E14" s="129" t="s">
+      <c r="I14" s="129" t="s">
         <v>519</v>
       </c>
-      <c r="F14" s="129" t="s">
-        <v>487</v>
-      </c>
-      <c r="G14" s="96" t="s">
-        <v>586</v>
-      </c>
-      <c r="H14" s="129" t="s">
+      <c r="J14" s="129" t="s">
         <v>520</v>
-      </c>
-      <c r="I14" s="129" t="s">
-        <v>521</v>
-      </c>
-      <c r="J14" s="129" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="140" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C15" s="129" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="129" t="s">
+        <v>521</v>
+      </c>
+      <c r="E15" s="129" t="s">
+        <v>522</v>
+      </c>
+      <c r="F15" s="129" t="s">
         <v>523</v>
       </c>
-      <c r="E15" s="129" t="s">
+      <c r="G15" s="96" t="s">
+        <v>582</v>
+      </c>
+      <c r="H15" s="129" t="s">
         <v>524</v>
       </c>
-      <c r="F15" s="129" t="s">
+      <c r="I15" s="129" t="s">
         <v>525</v>
       </c>
-      <c r="G15" s="96" t="s">
-        <v>585</v>
-      </c>
-      <c r="H15" s="129" t="s">
+      <c r="J15" s="129" t="s">
         <v>526</v>
-      </c>
-      <c r="I15" s="129" t="s">
-        <v>527</v>
-      </c>
-      <c r="J15" s="129" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="140" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C16" s="129" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="129" t="s">
+        <v>529</v>
+      </c>
+      <c r="E16" s="129" t="s">
+        <v>530</v>
+      </c>
+      <c r="F16" s="129" t="s">
+        <v>485</v>
+      </c>
+      <c r="G16" s="96" t="s">
+        <v>492</v>
+      </c>
+      <c r="H16" s="129" t="s">
         <v>531</v>
       </c>
-      <c r="E16" s="129" t="s">
+      <c r="I16" s="129" t="s">
         <v>532</v>
       </c>
-      <c r="F16" s="129" t="s">
-        <v>487</v>
-      </c>
-      <c r="G16" s="96" t="s">
-        <v>494</v>
-      </c>
-      <c r="H16" s="129" t="s">
-        <v>533</v>
-      </c>
-      <c r="I16" s="129" t="s">
-        <v>534</v>
-      </c>
       <c r="J16" s="129" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B17" s="145" t="s">
+        <v>359</v>
+      </c>
+      <c r="C17" s="152" t="s">
+        <v>308</v>
+      </c>
+      <c r="D17" s="146" t="s">
+        <v>508</v>
+      </c>
+      <c r="E17" s="147" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="145" t="s">
-        <v>361</v>
-      </c>
-      <c r="C17" s="152" t="s">
-        <v>310</v>
-      </c>
-      <c r="D17" s="146" t="s">
-        <v>510</v>
-      </c>
-      <c r="E17" s="147" t="s">
-        <v>511</v>
-      </c>
       <c r="F17" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G17" s="96"/>
       <c r="H17" s="129"/>
       <c r="I17" s="129"/>
       <c r="J17" s="129"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="140" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C18" s="129" t="s">
+        <v>510</v>
+      </c>
+      <c r="D18" s="129" t="s">
+        <v>511</v>
+      </c>
+      <c r="E18" s="129" t="s">
         <v>512</v>
       </c>
-      <c r="D18" s="129" t="s">
-        <v>513</v>
-      </c>
-      <c r="E18" s="129" t="s">
-        <v>514</v>
-      </c>
       <c r="F18" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G18" s="96"/>
       <c r="H18" s="129"/>
       <c r="I18" s="129"/>
       <c r="J18" s="129"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="140" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C19" s="129" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E19" s="129" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F19" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G19" s="96"/>
       <c r="H19" s="129"/>
       <c r="I19" s="129"/>
       <c r="J19" s="129"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" s="140" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C20" s="129" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E20" s="129" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F20" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G20" s="96"/>
       <c r="H20" s="129"/>
       <c r="I20" s="129"/>
       <c r="J20" s="129"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="135" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C21" s="136"/>
       <c r="D21" s="136"/>
       <c r="E21" s="136"/>
       <c r="F21" s="136"/>
       <c r="G21" s="93" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="H21" s="136" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="I21" s="136" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="J21" s="136" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="133" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C22" s="129"/>
       <c r="D22" s="129"/>
@@ -6292,201 +6374,208 @@
       <c r="I22" s="129"/>
       <c r="J22" s="129"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="140" t="s">
+        <v>365</v>
+      </c>
+      <c r="C23" s="129" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" s="129" t="s">
+        <v>540</v>
+      </c>
+      <c r="E23" s="129" t="s">
+        <v>519</v>
+      </c>
+      <c r="F23" s="129" t="s">
+        <v>541</v>
+      </c>
+      <c r="G23" s="96" t="s">
+        <v>542</v>
+      </c>
+      <c r="H23" s="129" t="s">
+        <v>543</v>
+      </c>
+      <c r="I23" s="129" t="s">
+        <v>544</v>
+      </c>
+      <c r="J23" s="129" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="145" t="s">
+        <v>366</v>
+      </c>
+      <c r="C24" s="152" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="146" t="s">
+        <v>546</v>
+      </c>
+      <c r="E24" s="147" t="s">
+        <v>509</v>
+      </c>
+      <c r="F24" s="146" t="s">
+        <v>547</v>
+      </c>
+      <c r="G24" s="96" t="s">
+        <v>548</v>
+      </c>
+      <c r="H24" s="129" t="s">
+        <v>549</v>
+      </c>
+      <c r="I24" s="129" t="s">
+        <v>550</v>
+      </c>
+      <c r="J24" s="129" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B25" s="140" t="s">
         <v>367</v>
       </c>
-      <c r="C23" s="129" t="s">
-        <v>221</v>
-      </c>
-      <c r="D23" s="129" t="s">
-        <v>542</v>
-      </c>
-      <c r="E23" s="129" t="s">
-        <v>521</v>
-      </c>
-      <c r="F23" s="129" t="s">
-        <v>543</v>
-      </c>
-      <c r="G23" s="96" t="s">
-        <v>544</v>
-      </c>
-      <c r="H23" s="129" t="s">
-        <v>545</v>
-      </c>
-      <c r="I23" s="129" t="s">
-        <v>546</v>
-      </c>
-      <c r="J23" s="129" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="145" t="s">
+      <c r="C25" s="129" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="129" t="s">
+        <v>554</v>
+      </c>
+      <c r="E25" s="129" t="s">
+        <v>555</v>
+      </c>
+      <c r="F25" s="129" t="s">
+        <v>485</v>
+      </c>
+      <c r="G25" s="96" t="s">
+        <v>556</v>
+      </c>
+      <c r="H25" s="129" t="s">
+        <v>557</v>
+      </c>
+      <c r="I25" s="129" t="s">
+        <v>558</v>
+      </c>
+      <c r="J25" s="129" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="145" t="s">
         <v>368</v>
       </c>
-      <c r="C24" s="152" t="s">
-        <v>292</v>
-      </c>
-      <c r="D24" s="146" t="s">
-        <v>548</v>
-      </c>
-      <c r="E24" s="147" t="s">
-        <v>511</v>
-      </c>
-      <c r="F24" s="146" t="s">
-        <v>549</v>
-      </c>
-      <c r="G24" s="96" t="s">
-        <v>550</v>
-      </c>
-      <c r="H24" s="129" t="s">
-        <v>551</v>
-      </c>
-      <c r="I24" s="129" t="s">
-        <v>552</v>
-      </c>
-      <c r="J24" s="129" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="140" t="s">
-        <v>369</v>
-      </c>
-      <c r="C25" s="129" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" s="129" t="s">
-        <v>556</v>
-      </c>
-      <c r="E25" s="129" t="s">
-        <v>557</v>
-      </c>
-      <c r="F25" s="129" t="s">
-        <v>487</v>
-      </c>
-      <c r="G25" s="96" t="s">
-        <v>558</v>
-      </c>
-      <c r="H25" s="129" t="s">
-        <v>559</v>
-      </c>
-      <c r="I25" s="129" t="s">
-        <v>560</v>
-      </c>
-      <c r="J25" s="129" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="145" t="s">
-        <v>370</v>
-      </c>
       <c r="C26" s="152" t="s">
+        <v>533</v>
+      </c>
+      <c r="D26" s="146" t="s">
+        <v>534</v>
+      </c>
+      <c r="E26" s="147" t="s">
         <v>535</v>
       </c>
-      <c r="D26" s="146" t="s">
-        <v>536</v>
-      </c>
-      <c r="E26" s="147" t="s">
-        <v>537</v>
-      </c>
       <c r="F26" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G26" s="96"/>
       <c r="H26" s="129"/>
       <c r="I26" s="129"/>
       <c r="J26" s="129"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="140" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C27" s="129" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D27" s="129" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E27" s="129" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F27" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G27" s="96"/>
       <c r="H27" s="129"/>
       <c r="I27" s="129"/>
       <c r="J27" s="129"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="140" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C28" s="96" t="s">
         <v>65</v>
       </c>
       <c r="D28" s="129" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E28" s="129" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F28" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G28" s="96"/>
       <c r="H28" s="129"/>
       <c r="I28" s="129"/>
       <c r="J28" s="129"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="140" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C29" s="129" t="s">
         <v>108</v>
       </c>
       <c r="D29" s="129" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E29" s="129" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F29" s="129" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G29" s="96"/>
       <c r="H29" s="129"/>
       <c r="I29" s="129"/>
       <c r="J29" s="129"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="158" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C30" s="136"/>
       <c r="D30" s="136"/>
       <c r="E30" s="136"/>
       <c r="F30" s="136"/>
       <c r="G30" s="105" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="H30" s="137" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="I30" s="138" t="s">
         <v>13</v>
       </c>
       <c r="J30" s="137" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+        <v>507</v>
+      </c>
+      <c r="M30" s="167" t="s">
+        <v>590</v>
+      </c>
+      <c r="N30" s="167"/>
+      <c r="O30" s="167"/>
+      <c r="P30" s="167"/>
+      <c r="Q30" s="167"/>
+    </row>
+    <row r="31" spans="2:17" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="133" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C31" s="129"/>
       <c r="D31" s="129"/>
@@ -6496,200 +6585,297 @@
       <c r="H31" s="129"/>
       <c r="I31" s="129"/>
       <c r="J31" s="129"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="M31" s="171" t="s">
+        <v>592</v>
+      </c>
+      <c r="N31" s="168" t="s">
+        <v>591</v>
+      </c>
+      <c r="P31" s="171" t="s">
+        <v>593</v>
+      </c>
+      <c r="Q31" s="168" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="145" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C32" s="148" t="s">
-        <v>111</v>
+        <v>596</v>
       </c>
       <c r="D32" s="146" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E32" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="146" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="G32" s="149" t="s">
-        <v>188</v>
+        <v>595</v>
       </c>
       <c r="H32" s="146" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="I32" s="147" t="s">
         <v>11</v>
       </c>
       <c r="J32" s="146" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+        <v>565</v>
+      </c>
+      <c r="M32" s="174">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="N32" s="168">
+        <f>1-(-M32)</f>
+        <v>0.86</v>
+      </c>
+      <c r="P32" s="172">
+        <v>-0.24</v>
+      </c>
+      <c r="Q32" s="170">
+        <f>1-(-P32)</f>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="145" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C33" s="148" t="s">
-        <v>111</v>
+        <v>596</v>
       </c>
       <c r="D33" s="146" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="E33" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="146" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="G33" s="149" t="s">
-        <v>569</v>
+        <v>59</v>
       </c>
       <c r="H33" s="146" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="I33" s="147" t="s">
         <v>11</v>
       </c>
       <c r="J33" s="146" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+      <c r="M33" s="174">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="N33" s="168">
+        <f t="shared" ref="N33:N38" si="0">1-(-M33)</f>
+        <v>0.86</v>
+      </c>
+      <c r="P33" s="172">
+        <v>-0.39</v>
+      </c>
+      <c r="Q33" s="170">
+        <f t="shared" ref="Q33:Q39" si="1">1-(-P33)</f>
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="145" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C34" s="148" t="s">
-        <v>65</v>
+        <v>598</v>
       </c>
       <c r="D34" s="146" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E34" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G34" s="149" t="s">
-        <v>111</v>
+        <v>596</v>
       </c>
       <c r="H34" s="146" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="I34" s="147" t="s">
         <v>11</v>
       </c>
       <c r="J34" s="146" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+        <v>507</v>
+      </c>
+      <c r="M34" s="174">
+        <v>-0.01</v>
+      </c>
+      <c r="N34" s="168">
+        <f t="shared" si="0"/>
+        <v>0.99</v>
+      </c>
+      <c r="P34" s="172">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="Q34" s="170">
+        <f t="shared" si="1"/>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="145" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C35" s="148" t="s">
-        <v>16</v>
+        <v>599</v>
       </c>
       <c r="D35" s="146" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E35" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G35" s="150"/>
       <c r="H35" s="129"/>
       <c r="I35" s="129"/>
       <c r="J35" s="129"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="M35" s="174">
+        <v>-0.06</v>
+      </c>
+      <c r="N35" s="168">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="P35" s="172"/>
+      <c r="Q35" s="170"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="145" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C36" s="149" t="s">
-        <v>478</v>
+        <v>600</v>
       </c>
       <c r="D36" s="146" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E36" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F36" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G36" s="150"/>
       <c r="H36" s="129"/>
       <c r="I36" s="129"/>
       <c r="J36" s="129"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="M36" s="172">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="N36" s="169">
+        <f t="shared" si="0"/>
+        <v>0.997</v>
+      </c>
+      <c r="P36" s="172"/>
+      <c r="Q36" s="170"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="145" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C37" s="148" t="s">
-        <v>195</v>
+        <v>601</v>
       </c>
       <c r="D37" s="146" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E37" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G37" s="150"/>
       <c r="H37" s="129"/>
       <c r="I37" s="129"/>
       <c r="J37" s="129"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="M37" s="174">
+        <v>-0.11</v>
+      </c>
+      <c r="N37" s="168">
+        <f t="shared" si="0"/>
+        <v>0.89</v>
+      </c>
+      <c r="P37" s="172"/>
+      <c r="Q37" s="170"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" s="145" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C38" s="148" t="s">
-        <v>512</v>
+        <v>602</v>
       </c>
       <c r="D38" s="146" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E38" s="147" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="146" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G38" s="150"/>
       <c r="H38" s="129"/>
       <c r="I38" s="129"/>
       <c r="J38" s="129"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="M38" s="174">
+        <v>-0.02</v>
+      </c>
+      <c r="N38" s="168">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="P38" s="172"/>
+      <c r="Q38" s="170"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="158" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C39" s="136"/>
       <c r="D39" s="136"/>
       <c r="E39" s="136"/>
       <c r="F39" s="136"/>
       <c r="G39" s="151" t="s">
-        <v>253</v>
+        <v>597</v>
       </c>
       <c r="H39" s="137" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="I39" s="138" t="s">
         <v>11</v>
       </c>
       <c r="J39" s="137" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>507</v>
+      </c>
+      <c r="P39" s="173">
+        <v>-0.15</v>
+      </c>
+      <c r="Q39" s="170">
+        <f t="shared" si="1"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="139" t="s">
         <v>19</v>
       </c>
@@ -6702,9 +6888,9 @@
       <c r="I40" s="129"/>
       <c r="J40" s="129"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="140" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C41" s="129" t="s">
         <v>100</v>
@@ -6713,32 +6899,32 @@
       <c r="E41" s="129"/>
       <c r="F41" s="129"/>
       <c r="G41" s="96" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="H41" s="129"/>
       <c r="I41" s="129"/>
       <c r="J41" s="129"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="140" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C42" s="129" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D42" s="129"/>
       <c r="E42" s="129"/>
       <c r="F42" s="129"/>
       <c r="G42" s="96" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="H42" s="129"/>
       <c r="I42" s="129"/>
       <c r="J42" s="129"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="82" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C43" s="157">
         <v>490</v>
@@ -6747,15 +6933,15 @@
       <c r="E43" s="129"/>
       <c r="F43" s="129"/>
       <c r="G43" s="96" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="H43" s="129"/>
       <c r="I43" s="129"/>
       <c r="J43" s="129"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" s="82" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C44" s="157">
         <v>28</v>
@@ -6764,13 +6950,13 @@
       <c r="E44" s="129"/>
       <c r="F44" s="129"/>
       <c r="G44" s="96" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H44" s="129"/>
       <c r="I44" s="129"/>
       <c r="J44" s="129"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="140" t="s">
         <v>21</v>
       </c>
@@ -6787,24 +6973,24 @@
       <c r="I45" s="129"/>
       <c r="J45" s="129"/>
     </row>
-    <row r="46" spans="2:10" ht="21" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17" ht="21" x14ac:dyDescent="0.2">
       <c r="B46" s="135" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C46" s="136" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D46" s="136"/>
       <c r="E46" s="136"/>
       <c r="F46" s="136"/>
       <c r="G46" s="93" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="H46" s="136"/>
       <c r="I46" s="136"/>
       <c r="J46" s="136"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" s="140"/>
       <c r="C47" s="129"/>
       <c r="D47" s="129"/>
@@ -6815,7 +7001,7 @@
       <c r="I47" s="129"/>
       <c r="J47" s="129"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" s="140"/>
       <c r="C48" s="129"/>
       <c r="D48" s="129"/>
@@ -6839,9 +7025,10 @@
     </row>
     <row r="53" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="M30:Q30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -6855,7 +7042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F98581C-D690-F849-931B-53E74322DAFE}">
   <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B40" sqref="B40:B41"/>
     </sheetView>
   </sheetViews>
@@ -6895,14 +7082,14 @@
       <c r="A2" s="81"/>
       <c r="B2" s="82"/>
       <c r="C2" s="165" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D2" s="165"/>
       <c r="E2" s="165"/>
       <c r="F2" s="165"/>
       <c r="G2" s="96"/>
       <c r="H2" s="166" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I2" s="166"/>
       <c r="J2" s="166"/>
@@ -6944,7 +7131,7 @@
     <row r="4" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="81"/>
       <c r="B4" s="89" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C4" s="86"/>
       <c r="D4" s="86"/>
@@ -6961,159 +7148,159 @@
     <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81"/>
       <c r="B5" s="82" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C5" s="83" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="83" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="83" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="F5" s="83" t="s">
         <v>222</v>
-      </c>
-      <c r="E5" s="83" t="s">
-        <v>223</v>
-      </c>
-      <c r="F5" s="83" t="s">
-        <v>224</v>
       </c>
       <c r="G5" s="96"/>
       <c r="H5" s="82" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I5" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J5" s="83" t="s">
+        <v>223</v>
+      </c>
+      <c r="K5" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="L5" s="83" t="s">
         <v>225</v>
-      </c>
-      <c r="K5" s="83" t="s">
-        <v>226</v>
-      </c>
-      <c r="L5" s="83" t="s">
-        <v>227</v>
       </c>
       <c r="M5" s="81"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="81"/>
       <c r="B6" s="82" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C6" s="83" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="E6" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="F6" s="83" t="s">
         <v>229</v>
-      </c>
-      <c r="E6" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="F6" s="83" t="s">
-        <v>231</v>
       </c>
       <c r="G6" s="96"/>
       <c r="H6" s="82" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I6" s="83" t="s">
+        <v>230</v>
+      </c>
+      <c r="J6" s="83" t="s">
+        <v>231</v>
+      </c>
+      <c r="K6" s="83" t="s">
         <v>232</v>
       </c>
-      <c r="J6" s="83" t="s">
+      <c r="L6" s="83" t="s">
         <v>233</v>
-      </c>
-      <c r="K6" s="83" t="s">
-        <v>234</v>
-      </c>
-      <c r="L6" s="83" t="s">
-        <v>235</v>
       </c>
       <c r="M6" s="81"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="81"/>
       <c r="B7" s="82" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C7" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="83" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>238</v>
+      </c>
+      <c r="F7" s="83" t="s">
         <v>239</v>
-      </c>
-      <c r="E7" s="83" t="s">
-        <v>240</v>
-      </c>
-      <c r="F7" s="83" t="s">
-        <v>241</v>
       </c>
       <c r="G7" s="96"/>
       <c r="H7" s="101" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I7" s="102" t="s">
+        <v>240</v>
+      </c>
+      <c r="J7" s="103" t="s">
+        <v>241</v>
+      </c>
+      <c r="K7" s="99" t="s">
         <v>242</v>
       </c>
-      <c r="J7" s="103" t="s">
+      <c r="L7" s="103" t="s">
         <v>243</v>
-      </c>
-      <c r="K7" s="99" t="s">
-        <v>244</v>
-      </c>
-      <c r="L7" s="103" t="s">
-        <v>245</v>
       </c>
       <c r="M7" s="81"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="81"/>
       <c r="B8" s="101" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C8" s="102" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D8" s="103" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E8" s="99" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="103" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G8" s="96"/>
       <c r="H8" s="101" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I8" s="102" t="s">
+        <v>336</v>
+      </c>
+      <c r="J8" s="103" t="s">
+        <v>337</v>
+      </c>
+      <c r="K8" s="99" t="s">
         <v>338</v>
       </c>
-      <c r="J8" s="103" t="s">
+      <c r="L8" s="103" t="s">
         <v>339</v>
-      </c>
-      <c r="K8" s="99" t="s">
-        <v>340</v>
-      </c>
-      <c r="L8" s="103" t="s">
-        <v>341</v>
       </c>
       <c r="M8" s="81"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="81"/>
       <c r="B9" s="101" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C9" s="102" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="103" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E9" s="99" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="103" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G9" s="96"/>
       <c r="H9" s="82"/>
@@ -7126,19 +7313,19 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="81"/>
       <c r="B10" s="82" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C10" s="83" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="83" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" s="83" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" s="83" t="s">
         <v>218</v>
-      </c>
-      <c r="E10" s="83" t="s">
-        <v>219</v>
-      </c>
-      <c r="F10" s="83" t="s">
-        <v>220</v>
       </c>
       <c r="G10" s="96"/>
       <c r="H10" s="82"/>
@@ -7151,19 +7338,19 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="81"/>
       <c r="B11" s="92" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C11" s="93" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="93" t="s">
+        <v>235</v>
+      </c>
+      <c r="F11" s="93" t="s">
         <v>236</v>
-      </c>
-      <c r="E11" s="93" t="s">
-        <v>237</v>
-      </c>
-      <c r="F11" s="93" t="s">
-        <v>238</v>
       </c>
       <c r="G11" s="96"/>
       <c r="H11" s="92"/>
@@ -7176,7 +7363,7 @@
     <row r="12" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="81"/>
       <c r="B12" s="89" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C12" s="83"/>
       <c r="D12" s="83"/>
@@ -7193,159 +7380,159 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="81"/>
       <c r="B13" s="82" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C13" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D13" s="83" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" s="83" t="s">
+        <v>255</v>
+      </c>
+      <c r="F13" s="83" t="s">
         <v>256</v>
-      </c>
-      <c r="E13" s="83" t="s">
-        <v>257</v>
-      </c>
-      <c r="F13" s="83" t="s">
-        <v>258</v>
       </c>
       <c r="G13" s="96"/>
       <c r="H13" s="101" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I13" s="102" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J13" s="103" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K13" s="99" t="s">
         <v>22</v>
       </c>
       <c r="L13" s="103" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="81"/>
       <c r="B14" s="82" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C14" s="83" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="83" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14" s="83" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" s="83" t="s">
         <v>261</v>
-      </c>
-      <c r="E14" s="83" t="s">
-        <v>262</v>
-      </c>
-      <c r="F14" s="83" t="s">
-        <v>263</v>
       </c>
       <c r="G14" s="96"/>
       <c r="H14" s="101" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="I14" s="102" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J14" s="103" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K14" s="99" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L14" s="103" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M14" s="81"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="81"/>
       <c r="B15" s="82" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C15" s="83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="83" t="s">
+        <v>267</v>
+      </c>
+      <c r="E15" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="F15" s="83" t="s">
         <v>269</v>
-      </c>
-      <c r="E15" s="83" t="s">
-        <v>270</v>
-      </c>
-      <c r="F15" s="83" t="s">
-        <v>271</v>
       </c>
       <c r="G15" s="96"/>
       <c r="H15" s="82" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I15" s="83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J15" s="83" t="s">
+        <v>270</v>
+      </c>
+      <c r="K15" s="83" t="s">
+        <v>271</v>
+      </c>
+      <c r="L15" s="83" t="s">
         <v>272</v>
-      </c>
-      <c r="K15" s="83" t="s">
-        <v>273</v>
-      </c>
-      <c r="L15" s="83" t="s">
-        <v>274</v>
       </c>
       <c r="M15" s="81"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="81"/>
       <c r="B16" s="82" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C16" s="83" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" s="83" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" s="83" t="s">
         <v>246</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="F16" s="83" t="s">
         <v>247</v>
-      </c>
-      <c r="E16" s="83" t="s">
-        <v>248</v>
-      </c>
-      <c r="F16" s="83" t="s">
-        <v>249</v>
       </c>
       <c r="G16" s="96"/>
       <c r="H16" s="82" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I16" s="83" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="83" t="s">
+        <v>340</v>
+      </c>
+      <c r="K16" s="83" t="s">
+        <v>341</v>
+      </c>
+      <c r="L16" s="83" t="s">
         <v>342</v>
-      </c>
-      <c r="K16" s="83" t="s">
-        <v>343</v>
-      </c>
-      <c r="L16" s="83" t="s">
-        <v>344</v>
       </c>
       <c r="M16" s="81"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="81"/>
       <c r="B17" s="82" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C17" s="83" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="83" t="s">
+        <v>248</v>
+      </c>
+      <c r="E17" s="83" t="s">
+        <v>249</v>
+      </c>
+      <c r="F17" s="83" t="s">
         <v>250</v>
-      </c>
-      <c r="E17" s="83" t="s">
-        <v>251</v>
-      </c>
-      <c r="F17" s="83" t="s">
-        <v>252</v>
       </c>
       <c r="G17" s="96"/>
       <c r="H17" s="82"/>
@@ -7358,19 +7545,19 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="81"/>
       <c r="B18" s="82" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C18" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="D18" s="83" t="s">
+        <v>252</v>
+      </c>
+      <c r="E18" s="83" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="83" t="s">
         <v>253</v>
-      </c>
-      <c r="D18" s="83" t="s">
-        <v>254</v>
-      </c>
-      <c r="E18" s="83" t="s">
-        <v>187</v>
-      </c>
-      <c r="F18" s="83" t="s">
-        <v>255</v>
       </c>
       <c r="G18" s="96"/>
       <c r="H18" s="82"/>
@@ -7383,19 +7570,19 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="81"/>
       <c r="B19" s="92" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C19" s="93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D19" s="93" t="s">
+        <v>264</v>
+      </c>
+      <c r="E19" s="93" t="s">
+        <v>265</v>
+      </c>
+      <c r="F19" s="93" t="s">
         <v>266</v>
-      </c>
-      <c r="E19" s="93" t="s">
-        <v>267</v>
-      </c>
-      <c r="F19" s="93" t="s">
-        <v>268</v>
       </c>
       <c r="G19" s="96"/>
       <c r="H19" s="92"/>
@@ -7409,7 +7596,7 @@
     <row r="20" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="81"/>
       <c r="B20" s="89" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C20" s="83"/>
       <c r="D20" s="83"/>
@@ -7427,159 +7614,159 @@
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="81"/>
       <c r="B21" s="82" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C21" s="83" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D21" s="83" t="s">
+        <v>283</v>
+      </c>
+      <c r="E21" s="83" t="s">
+        <v>284</v>
+      </c>
+      <c r="F21" s="83" t="s">
         <v>285</v>
-      </c>
-      <c r="E21" s="83" t="s">
-        <v>286</v>
-      </c>
-      <c r="F21" s="83" t="s">
-        <v>287</v>
       </c>
       <c r="G21" s="96"/>
       <c r="H21" s="82" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I21" s="83" t="s">
+        <v>286</v>
+      </c>
+      <c r="J21" s="83" t="s">
+        <v>287</v>
+      </c>
+      <c r="K21" s="83" t="s">
         <v>288</v>
       </c>
-      <c r="J21" s="83" t="s">
+      <c r="L21" s="83" t="s">
         <v>289</v>
-      </c>
-      <c r="K21" s="83" t="s">
-        <v>290</v>
-      </c>
-      <c r="L21" s="83" t="s">
-        <v>291</v>
       </c>
       <c r="M21" s="81"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="81"/>
       <c r="B22" s="82" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C22" s="83" t="s">
+        <v>290</v>
+      </c>
+      <c r="D22" s="83" t="s">
+        <v>291</v>
+      </c>
+      <c r="E22" s="83" t="s">
         <v>292</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="F22" s="83" t="s">
         <v>293</v>
-      </c>
-      <c r="E22" s="83" t="s">
-        <v>294</v>
-      </c>
-      <c r="F22" s="83" t="s">
-        <v>295</v>
       </c>
       <c r="G22" s="96"/>
       <c r="H22" s="82" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I22" s="83" t="s">
+        <v>294</v>
+      </c>
+      <c r="J22" s="83" t="s">
+        <v>295</v>
+      </c>
+      <c r="K22" s="83" t="s">
         <v>296</v>
       </c>
-      <c r="J22" s="83" t="s">
+      <c r="L22" s="83" t="s">
         <v>297</v>
-      </c>
-      <c r="K22" s="83" t="s">
-        <v>298</v>
-      </c>
-      <c r="L22" s="83" t="s">
-        <v>299</v>
       </c>
       <c r="M22" s="81"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="81"/>
       <c r="B23" s="82" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C23" s="83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D23" s="83" t="s">
+        <v>301</v>
+      </c>
+      <c r="E23" s="83" t="s">
+        <v>302</v>
+      </c>
+      <c r="F23" s="83" t="s">
         <v>303</v>
-      </c>
-      <c r="E23" s="83" t="s">
-        <v>304</v>
-      </c>
-      <c r="F23" s="83" t="s">
-        <v>305</v>
       </c>
       <c r="G23" s="96"/>
       <c r="H23" s="82" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I23" s="83" t="s">
+        <v>304</v>
+      </c>
+      <c r="J23" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="K23" s="83" t="s">
         <v>306</v>
       </c>
-      <c r="J23" s="83" t="s">
+      <c r="L23" s="83" t="s">
         <v>307</v>
-      </c>
-      <c r="K23" s="83" t="s">
-        <v>308</v>
-      </c>
-      <c r="L23" s="83" t="s">
-        <v>309</v>
       </c>
       <c r="M23" s="81"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="81"/>
       <c r="B24" s="82" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C24" s="83" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="83" t="s">
+        <v>273</v>
+      </c>
+      <c r="E24" s="83" t="s">
+        <v>274</v>
+      </c>
+      <c r="F24" s="83" t="s">
         <v>275</v>
-      </c>
-      <c r="E24" s="83" t="s">
-        <v>276</v>
-      </c>
-      <c r="F24" s="83" t="s">
-        <v>277</v>
       </c>
       <c r="G24" s="96"/>
       <c r="H24" s="101" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I24" s="102" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J24" s="103" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K24" s="99" t="s">
         <v>14</v>
       </c>
       <c r="L24" s="103" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="M24" s="81"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="81"/>
       <c r="B25" s="82" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C25" s="83" t="s">
+        <v>276</v>
+      </c>
+      <c r="D25" s="83" t="s">
+        <v>277</v>
+      </c>
+      <c r="E25" s="83" t="s">
         <v>278</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="F25" s="83" t="s">
         <v>279</v>
-      </c>
-      <c r="E25" s="83" t="s">
-        <v>280</v>
-      </c>
-      <c r="F25" s="83" t="s">
-        <v>281</v>
       </c>
       <c r="G25" s="96"/>
       <c r="H25" s="82"/>
@@ -7592,19 +7779,19 @@
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="81"/>
       <c r="B26" s="82" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C26" s="83" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="83" t="s">
+        <v>280</v>
+      </c>
+      <c r="E26" s="83" t="s">
+        <v>281</v>
+      </c>
+      <c r="F26" s="83" t="s">
         <v>282</v>
-      </c>
-      <c r="E26" s="83" t="s">
-        <v>283</v>
-      </c>
-      <c r="F26" s="83" t="s">
-        <v>284</v>
       </c>
       <c r="G26" s="96"/>
       <c r="H26" s="82"/>
@@ -7617,19 +7804,19 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="81"/>
       <c r="B27" s="92" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C27" s="93" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D27" s="93" t="s">
+        <v>298</v>
+      </c>
+      <c r="E27" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="F27" s="93" t="s">
         <v>300</v>
-      </c>
-      <c r="E27" s="93" t="s">
-        <v>301</v>
-      </c>
-      <c r="F27" s="93" t="s">
-        <v>302</v>
       </c>
       <c r="G27" s="96"/>
       <c r="H27" s="92"/>
@@ -7642,7 +7829,7 @@
     <row r="28" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="81"/>
       <c r="B28" s="89" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C28" s="83"/>
       <c r="D28" s="83"/>
@@ -7659,102 +7846,102 @@
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="81"/>
       <c r="B29" s="101" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C29" s="102" t="s">
         <v>57</v>
       </c>
       <c r="D29" s="103" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E29" s="99" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="103" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G29" s="96"/>
       <c r="H29" s="101" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I29" s="102" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J29" s="103" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K29" s="99" t="s">
         <v>11</v>
       </c>
       <c r="L29" s="103" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="M29" s="81"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="81"/>
       <c r="B30" s="101" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C30" s="102" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D30" s="103" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E30" s="99" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="103" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G30" s="96"/>
       <c r="H30" s="101" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I30" s="102" t="s">
+        <v>325</v>
+      </c>
+      <c r="J30" s="103" t="s">
+        <v>326</v>
+      </c>
+      <c r="K30" s="99" t="s">
         <v>327</v>
       </c>
-      <c r="J30" s="103" t="s">
+      <c r="L30" s="103" t="s">
         <v>328</v>
-      </c>
-      <c r="K30" s="99" t="s">
-        <v>329</v>
-      </c>
-      <c r="L30" s="103" t="s">
-        <v>330</v>
       </c>
       <c r="M30" s="81"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="81"/>
       <c r="B31" s="101" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C31" s="102" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D31" s="103" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E31" s="99" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="103" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G31" s="96"/>
       <c r="H31" s="82" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I31" s="83" t="s">
         <v>17</v>
       </c>
       <c r="J31" s="83" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K31" s="83" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L31" s="83">
         <v>44742</v>
@@ -7764,54 +7951,54 @@
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="81"/>
       <c r="B32" s="101" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C32" s="102" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D32" s="103" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E32" s="99" t="s">
         <v>13</v>
       </c>
       <c r="F32" s="103" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G32" s="96"/>
       <c r="H32" s="101" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I32" s="102" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J32" s="103" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K32" s="99" t="s">
         <v>11</v>
       </c>
       <c r="L32" s="103" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="M32" s="81"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="81"/>
       <c r="B33" s="101" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C33" s="102" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D33" s="103" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E33" s="99" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="103" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G33" s="96"/>
       <c r="H33" s="82"/>
@@ -7824,19 +8011,19 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="81"/>
       <c r="B34" s="101" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C34" s="102" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D34" s="103" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E34" s="99" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G34" s="96"/>
       <c r="H34" s="82"/>
@@ -7849,19 +8036,19 @@
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="81"/>
       <c r="B35" s="104" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C35" s="105" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D35" s="106" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E35" s="100" t="s">
         <v>110</v>
       </c>
       <c r="F35" s="106" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G35" s="96"/>
       <c r="H35" s="92"/>
@@ -7891,10 +8078,10 @@
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="81"/>
       <c r="B37" s="82" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C37" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D37" s="83"/>
       <c r="E37" s="83"/>
@@ -7902,7 +8089,7 @@
       <c r="G37" s="96"/>
       <c r="H37" s="82"/>
       <c r="I37" s="83" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J37" s="83"/>
       <c r="K37" s="83"/>
@@ -7912,10 +8099,10 @@
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="81"/>
       <c r="B38" s="82" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C38" s="83" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D38" s="83"/>
       <c r="E38" s="83"/>
@@ -7923,7 +8110,7 @@
       <c r="G38" s="96"/>
       <c r="H38" s="82"/>
       <c r="I38" s="83" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J38" s="83"/>
       <c r="K38" s="83"/>
@@ -7933,10 +8120,10 @@
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="81"/>
       <c r="B39" s="82" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C39" s="83" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D39" s="83"/>
       <c r="E39" s="83"/>
@@ -7944,7 +8131,7 @@
       <c r="G39" s="96"/>
       <c r="H39" s="82"/>
       <c r="I39" s="83" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J39" s="83"/>
       <c r="K39" s="83"/>
@@ -7954,10 +8141,10 @@
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="81"/>
       <c r="B40" s="82" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C40" s="83" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D40" s="83"/>
       <c r="E40" s="83"/>
@@ -7965,7 +8152,7 @@
       <c r="G40" s="96"/>
       <c r="H40" s="82"/>
       <c r="I40" s="83" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J40" s="83"/>
       <c r="K40" s="83"/>
@@ -7975,10 +8162,10 @@
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="81"/>
       <c r="B41" s="82" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C41" s="83" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D41" s="83"/>
       <c r="E41" s="83"/>
@@ -7986,7 +8173,7 @@
       <c r="G41" s="96"/>
       <c r="H41" s="82"/>
       <c r="I41" s="83" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J41" s="83"/>
       <c r="K41" s="83"/>
@@ -8017,10 +8204,10 @@
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="81"/>
       <c r="B43" s="92" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C43" s="93" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D43" s="93"/>
       <c r="E43" s="93"/>
@@ -8028,7 +8215,7 @@
       <c r="G43" s="93"/>
       <c r="H43" s="92"/>
       <c r="I43" s="93" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J43" s="93"/>
       <c r="K43" s="93"/>
@@ -8098,7 +8285,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -8124,13 +8311,13 @@
       <c r="A2" s="87"/>
       <c r="B2" s="94"/>
       <c r="C2" s="107" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D2" s="107" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E2" s="107" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F2" s="107" t="s">
         <v>3</v>
@@ -8141,7 +8328,7 @@
     <row r="3" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="87"/>
       <c r="B3" s="112" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C3" s="83"/>
       <c r="D3" s="83"/>
@@ -8153,7 +8340,7 @@
     <row r="4" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="87"/>
       <c r="B4" s="88" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C4" s="83"/>
       <c r="D4" s="83"/>
@@ -8165,19 +8352,19 @@
     <row r="5" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="87"/>
       <c r="B5" s="108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="83" t="s">
+        <v>459</v>
+      </c>
+      <c r="D5" s="83" t="s">
+        <v>460</v>
+      </c>
+      <c r="E5" s="83" t="s">
         <v>461</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="F5" s="84" t="s">
         <v>462</v>
-      </c>
-      <c r="E5" s="83" t="s">
-        <v>463</v>
-      </c>
-      <c r="F5" s="84" t="s">
-        <v>464</v>
       </c>
       <c r="G5" s="87"/>
       <c r="H5" s="87"/>
@@ -8185,16 +8372,16 @@
     <row r="6" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="87"/>
       <c r="B6" s="110" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C6" s="103" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="103" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E6" s="103" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F6" s="99" t="s">
         <v>14</v>
@@ -8205,16 +8392,16 @@
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="87"/>
       <c r="B7" s="110" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C7" s="103" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="103" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E7" s="103" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F7" s="99" t="s">
         <v>14</v>
@@ -8225,7 +8412,7 @@
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="87"/>
       <c r="B8" s="88" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C8" s="83"/>
       <c r="D8" s="83"/>
@@ -8238,16 +8425,16 @@
     <row r="9" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="87"/>
       <c r="B9" s="108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="83" t="s">
+        <v>465</v>
+      </c>
+      <c r="D9" s="83" t="s">
+        <v>466</v>
+      </c>
+      <c r="E9" s="83" t="s">
         <v>467</v>
-      </c>
-      <c r="D9" s="83" t="s">
-        <v>468</v>
-      </c>
-      <c r="E9" s="83" t="s">
-        <v>469</v>
       </c>
       <c r="F9" s="84" t="s">
         <v>22</v>
@@ -8258,19 +8445,19 @@
     <row r="10" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="87"/>
       <c r="B10" s="110" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C10" s="103" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D10" s="103" t="s">
         <v>110</v>
       </c>
       <c r="E10" s="103" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F10" s="99" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G10" s="87"/>
       <c r="H10" s="87"/>
@@ -8278,16 +8465,16 @@
     <row r="11" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="87"/>
       <c r="B11" s="111" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C11" s="106" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D11" s="106" t="s">
         <v>110</v>
       </c>
       <c r="E11" s="106" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F11" s="100" t="s">
         <v>13</v>
@@ -8298,7 +8485,7 @@
     <row r="12" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="87"/>
       <c r="B12" s="112" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C12" s="83"/>
       <c r="D12" s="83"/>
@@ -8310,7 +8497,7 @@
     <row r="13" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="87"/>
       <c r="B13" s="88" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C13" s="83"/>
       <c r="D13" s="83"/>
@@ -8322,19 +8509,19 @@
     <row r="14" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="87"/>
       <c r="B14" s="108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="83" t="s">
+        <v>472</v>
+      </c>
+      <c r="D14" s="83" t="s">
+        <v>473</v>
+      </c>
+      <c r="E14" s="83" t="s">
         <v>474</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="F14" s="83" t="s">
         <v>475</v>
-      </c>
-      <c r="E14" s="83" t="s">
-        <v>476</v>
-      </c>
-      <c r="F14" s="83" t="s">
-        <v>477</v>
       </c>
       <c r="G14" s="87"/>
       <c r="H14" s="87"/>
@@ -8342,19 +8529,19 @@
     <row r="15" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="87"/>
       <c r="B15" s="108" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C15" s="83" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E15" s="83" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F15" s="83" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G15" s="87"/>
       <c r="H15" s="87"/>
@@ -8362,19 +8549,19 @@
     <row r="16" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="87"/>
       <c r="B16" s="108" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C16" s="83" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D16" s="83" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E16" s="83" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F16" s="83" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G16" s="87"/>
       <c r="H16" s="87"/>
@@ -8382,7 +8569,7 @@
     <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="87"/>
       <c r="B17" s="88" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C17" s="83"/>
       <c r="D17" s="83"/>
@@ -8394,19 +8581,19 @@
     <row r="18" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="87"/>
       <c r="B18" s="108" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="83" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D18" s="83" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E18" s="83" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F18" s="83" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G18" s="87"/>
       <c r="H18" s="87"/>
@@ -8414,19 +8601,19 @@
     <row r="19" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="87"/>
       <c r="B19" s="108" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C19" s="83" t="s">
+        <v>479</v>
+      </c>
+      <c r="D19" s="83" t="s">
+        <v>278</v>
+      </c>
+      <c r="E19" s="83" t="s">
+        <v>480</v>
+      </c>
+      <c r="F19" s="83" t="s">
         <v>481</v>
-      </c>
-      <c r="D19" s="83" t="s">
-        <v>280</v>
-      </c>
-      <c r="E19" s="83" t="s">
-        <v>482</v>
-      </c>
-      <c r="F19" s="83" t="s">
-        <v>483</v>
       </c>
       <c r="G19" s="87"/>
       <c r="H19" s="87"/>
@@ -8434,19 +8621,19 @@
     <row r="20" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="87"/>
       <c r="B20" s="109" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C20" s="93" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D20" s="93" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E20" s="93" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F20" s="93" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G20" s="87"/>
       <c r="H20" s="87"/>
@@ -8522,13 +8709,13 @@
       <c r="A3" s="120"/>
       <c r="B3" s="121"/>
       <c r="C3" s="107" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D3" s="107" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E3" s="107" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F3" s="122" t="s">
         <v>3</v>
@@ -8539,7 +8726,7 @@
     <row r="4" spans="1:8" s="113" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="123"/>
       <c r="B4" s="117" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C4" s="127"/>
       <c r="D4" s="127"/>
@@ -8550,16 +8737,16 @@
     <row r="5" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="120"/>
       <c r="B5" s="118" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C5" s="83" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D5" s="83" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E5" s="83" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F5" s="125" t="s">
         <v>11</v>
@@ -8569,16 +8756,16 @@
     <row r="6" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="120"/>
       <c r="B6" s="118" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C6" s="83" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D6" s="83" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E6" s="83" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F6" s="125" t="s">
         <v>17</v>
@@ -8588,16 +8775,16 @@
     <row r="7" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="120"/>
       <c r="B7" s="118" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C7" s="83" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D7" s="83" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E7" s="83" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F7" s="125" t="s">
         <v>11</v>
@@ -8607,73 +8794,73 @@
     <row r="8" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="120"/>
       <c r="B8" s="118" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C8" s="83" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D8" s="83" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E8" s="83" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F8" s="119" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G8" s="120"/>
     </row>
     <row r="9" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="120"/>
       <c r="B9" s="118" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C9" s="83" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D9" s="83" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E9" s="83" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F9" s="119" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G9" s="120"/>
     </row>
     <row r="10" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="120"/>
       <c r="B10" s="118" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C10" s="83" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D10" s="83" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E10" s="83" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F10" s="128" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G10" s="120"/>
     </row>
     <row r="11" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="120"/>
       <c r="B11" s="121" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C11" s="93" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D11" s="93" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E11" s="93" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F11" s="75" t="s">
         <v>17</v>
@@ -8683,7 +8870,7 @@
     <row r="12" spans="1:8" s="113" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="123"/>
       <c r="B12" s="117" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C12" s="127"/>
       <c r="D12" s="127"/>
@@ -8694,76 +8881,76 @@
     <row r="13" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="120"/>
       <c r="B13" s="118" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C13" s="83" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D13" s="83" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E13" s="83" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F13" s="119" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G13" s="120"/>
     </row>
     <row r="14" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="120"/>
       <c r="B14" s="118" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C14" s="83" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D14" s="83" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E14" s="83" t="s">
+        <v>455</v>
+      </c>
+      <c r="F14" s="119" t="s">
         <v>457</v>
-      </c>
-      <c r="F14" s="119" t="s">
-        <v>459</v>
       </c>
       <c r="G14" s="120"/>
     </row>
     <row r="15" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="120"/>
       <c r="B15" s="118" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C15" s="83" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D15" s="83" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E15" s="83" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F15" s="119" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G15" s="120"/>
     </row>
     <row r="16" spans="1:8" s="114" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="120"/>
       <c r="B16" s="121" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D16" s="93" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E16" s="93" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F16" s="126" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G16" s="120"/>
     </row>
@@ -8800,7 +8987,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8824,33 +9011,33 @@
         <v>68</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E2" s="56"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="56"/>
       <c r="B3" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E3" s="56"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="56"/>
       <c r="B4" s="49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" s="55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" s="56"/>
     </row>
@@ -8858,17 +9045,17 @@
       <c r="A5" s="56"/>
       <c r="B5" s="46"/>
       <c r="C5" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="48" t="s">
         <v>144</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>145</v>
       </c>
       <c r="E5" s="56"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="56"/>
       <c r="B6" s="49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
@@ -8877,23 +9064,23 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="56"/>
       <c r="B7" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="56"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="56"/>
       <c r="B8" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" s="48" t="s">
         <v>71</v>
@@ -8903,26 +9090,26 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="56"/>
       <c r="B9" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="56"/>
       <c r="B10" s="51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" s="56"/>
     </row>

</xml_diff>